<commit_message>
add block diagrams, better graph in xlsx
</commit_message>
<xml_diff>
--- a/Figure8.xlsx
+++ b/Figure8.xlsx
@@ -116,38 +116,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -5053,16 +5022,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>